<commit_message>
Added Colosseum Game PDF
</commit_message>
<xml_diff>
--- a/Arena of the Eternal Knight.xlsx
+++ b/Arena of the Eternal Knight.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2973742c209d6a4f/Desktop/Concept/concept25-JakeReid22/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2973742c209d6a4f/Desktop/New folder/concept25-JakeReid22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{7216789F-CD0B-4CE4-BB9A-411AEA21EADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE3B7549-301D-4E80-899E-1A94276FD165}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{7216789F-CD0B-4CE4-BB9A-411AEA21EADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D95AA132-C6D9-4C63-970A-EC5B11DC5C9D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{B114BF61-C9F1-47F8-B51B-C5362F104DFD}"/>
   </bookViews>
@@ -141,9 +141,6 @@
     <t>Team Member B</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
     <t>Team Member C</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tried to save it on the actual one but it wont save my edits, I'm going to try save it on to it when I go into college this week </t>
+  </si>
+  <si>
+    <t>Cormac Bowes</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,7 +627,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1"/>
       <c r="N1" s="10">
@@ -1211,7 +1211,7 @@
         <v>33</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -1219,50 +1219,50 @@
         <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>